<commit_message>
Arunkumar K: Added new testcases from Abirami and created automation for HomePage
</commit_message>
<xml_diff>
--- a/TAP_POM_Framework/data/TC003.xlsx
+++ b/TAP_POM_Framework/data/TC003.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="7845"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -39,35 +40,43 @@
     <t>Password</t>
   </si>
   <si>
-    <t>SampleCompany</t>
-  </si>
-  <si>
-    <t>www.samplecompany.com</t>
-  </si>
-  <si>
     <t>Sam</t>
   </si>
   <si>
     <t>Weber</t>
   </si>
   <si>
-    <t>Sam@sc.com</t>
-  </si>
-  <si>
     <t>Samuel@123</t>
   </si>
   <si>
-    <t>+145 326-5867</t>
+    <t>SampleCompany1</t>
+  </si>
+  <si>
+    <t>213213216546</t>
+  </si>
+  <si>
+    <t>Sam@sc1.com</t>
+  </si>
+  <si>
+    <t>www.samplecompany1.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,16 +105,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,7 +457,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,25 +496,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>